<commit_message>
simulations complete for AA1000, AA2024, AA5000, AA6000, AA7075, Al
</commit_message>
<xml_diff>
--- a/data/averaged_filtered_AA5000.xlsx
+++ b/data/averaged_filtered_AA5000.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F91"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,485 +468,1981 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>C1=CC(=C(C(=C1)C=NC2=CC=C(C=C2)N=CC3=CC=CC(=C3O)OC)O)OC</t>
+          <t>C(C(=O)[O-])C(CC(=O)[O-])(C(=O)[O-])O</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2</v>
+        <v>0.33</v>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="D2" t="n">
-        <v>0.0003</v>
+        <v>0.0045</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>59.125</v>
+        <v>77.90000000000001</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>C1=CC(=C(C(=C1)C=NC2=CC=C(C=C2)N=CC3=CC=CC(=C3O)OC)O)OC</t>
+          <t>C(C(=O)[O-])C(CC(=O)[O-])(C(=O)[O-])O</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>2</v>
+        <v>0.33</v>
       </c>
       <c r="C3" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="D3" t="n">
-        <v>0.0005</v>
+        <v>0.02</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>67.375</v>
+        <v>99.90000000000001</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>C1=CC(=C(C(=C1)C=NC2=CC=C(C=C2)N=CC3=CC=CC(=C3O)OC)O)OC</t>
+          <t>C(C(=O)[O-])C(CC(=O)[O-])(C(=O)[O-])O</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>2</v>
+        <v>0.58</v>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="D4" t="n">
-        <v>0.0008</v>
+        <v>0.0045</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>74.125</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>C1=CC(=C(C(=C1)C=NC2=CC=C(C=C2)N=CC3=CC=CC(=C3O)OC)O)OC</t>
+          <t>C(C(=O)[O-])C(CC(=O)[O-])(C(=O)[O-])O</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>2</v>
+        <v>1.67</v>
       </c>
       <c r="C5" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="D5" t="n">
-        <v>0.001</v>
+        <v>0.002</v>
       </c>
       <c r="E5" t="n">
         <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>77</v>
+        <v>35.23333333333333</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>C1=CC(=C(C(=C1)C=NC2=CC=C(C=C2)N=CC3=CC=CC(=C3O)OC)O)OC</t>
+          <t>C(C(=O)[O-])C(CC(=O)[O-])(C(=O)[O-])O</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>2</v>
+        <v>1.67</v>
       </c>
       <c r="C6" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="D6" t="n">
-        <v>0.0013</v>
+        <v>0.0045</v>
       </c>
       <c r="E6" t="n">
         <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>81.5</v>
+        <v>76.2</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>C1=CC(=C(C(=C1)C=NC2=CC=C(C=C2)N=CC3=CC=CC(=C3O)OC)O)OC</t>
+          <t>C(C(=O)[O-])C(CC(=O)[O-])(C(=O)[O-])O</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>4</v>
+        <v>1.67</v>
       </c>
       <c r="C7" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="D7" t="n">
-        <v>0.0013</v>
+        <v>0.007</v>
       </c>
       <c r="E7" t="n">
         <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>85</v>
+        <v>93.36666666666667</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>C1=CC(=C(C(=C1)C=NC2=CC=C(C=C2)N=CC3=CC=CC(=C3O)OC)O)OC</t>
+          <t>C(C(=O)[O-])C(CC(=O)[O-])(C(=O)[O-])O</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>6</v>
+        <v>1.67</v>
       </c>
       <c r="C8" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="D8" t="n">
-        <v>0.0013</v>
+        <v>0.008999999999999999</v>
       </c>
       <c r="E8" t="n">
         <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>81.5</v>
+        <v>98.96666666666665</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>C1=CC(=C(C(=C1)C=NC2=CC=C(C=C2)N=CC3=CC=CC(=C3O)OC)O)OC</t>
+          <t>C(C(=O)[O-])C(CC(=O)[O-])(C(=O)[O-])O</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>8</v>
+        <v>1.67</v>
       </c>
       <c r="C9" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="D9" t="n">
-        <v>0.0013</v>
+        <v>0.02</v>
       </c>
       <c r="E9" t="n">
         <v>0</v>
       </c>
       <c r="F9" t="n">
-        <v>73.5</v>
+        <v>99.825</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>C1=CC(=C(C(=C1)C=NC2=CC=C(C=C2)N=CC3=CC=CC(=C3O)OC)O)OC</t>
+          <t>C1=CC(=C(C=C1Cl)Cl)COC(CN2C=CN=C2)C3=C(C=C(C=C3)Cl)Cl.[N+](=O)(O)[O-]</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>24</v>
+        <v>336</v>
       </c>
       <c r="C10" t="n">
-        <v>0</v>
+        <v>4.6</v>
       </c>
       <c r="D10" t="n">
-        <v>0.0013</v>
+        <v>0.00021</v>
       </c>
       <c r="E10" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="F10" t="n">
-        <v>21</v>
+        <v>59.05</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>C1=CC(=CN=C1)C(=O)NN</t>
+          <t>C1=CC(=C(C=C1Cl)Cl)COC(CN2C=CN=C2)C3=C(C=C(C=C3)Cl)Cl.[N+](=O)(O)[O-]</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>4</v>
+        <v>336</v>
       </c>
       <c r="C11" t="n">
-        <v>0</v>
+        <v>7.6</v>
       </c>
       <c r="D11" t="n">
-        <v>6.999999999999999e-05</v>
+        <v>0.00042</v>
       </c>
       <c r="E11" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="F11" t="n">
-        <v>75.15333333333332</v>
+        <v>94</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>C1=CC(=CN=C1)C(=O)NN</t>
+          <t>C1=CC(=C(C=C1Cl)Cl)COC(CN2C=CN=C2)C3=C(C=C(C=C3)Cl)Cl.[N+](=O)(O)[O-]</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>4</v>
+        <v>336</v>
       </c>
       <c r="C12" t="n">
-        <v>0</v>
+        <v>7.6</v>
       </c>
       <c r="D12" t="n">
-        <v>0.0004</v>
+        <v>0.00084</v>
       </c>
       <c r="E12" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="F12" t="n">
-        <v>72.80666666666667</v>
+        <v>96.40000000000001</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>C1=CC(=CN=C1)C(=O)NN</t>
+          <t>C1=CC(=CC(=C1)O)O</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="C13" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="D13" t="n">
-        <v>0.0007</v>
+        <v>0.001</v>
       </c>
       <c r="E13" t="n">
         <v>0</v>
       </c>
       <c r="F13" t="n">
-        <v>74.08666666666666</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>C1=CC(=CN=C1)C(=O)NN</t>
+          <t>C1=CC(=CC(=C1)O)O</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="C14" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="D14" t="n">
-        <v>0.0018</v>
+        <v>0.01</v>
       </c>
       <c r="E14" t="n">
         <v>0</v>
       </c>
       <c r="F14" t="n">
-        <v>75.26333333333334</v>
+        <v>53.3</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>C1=CC=C(C(=C1)C=NC2=CC=C(C=C2)N=CC3=CC=CC=C3O)O</t>
+          <t>C1=CC(=CC(=C1)O)O</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="C15" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="D15" t="n">
-        <v>0.0003</v>
+        <v>0.1</v>
       </c>
       <c r="E15" t="n">
         <v>0</v>
       </c>
       <c r="F15" t="n">
-        <v>56.625</v>
+        <v>98.7</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>C1=CC=C(C(=C1)C=NC2=CC=C(C=C2)N=CC3=CC=CC=C3O)O</t>
+          <t>C1=CC(=CC=C1O)O</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="C16" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="D16" t="n">
-        <v>0.0005999999999999999</v>
+        <v>0.001</v>
       </c>
       <c r="E16" t="n">
         <v>0</v>
       </c>
       <c r="F16" t="n">
-        <v>62</v>
+        <v>64.09999999999999</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>C1=CC=C(C(=C1)C=NC2=CC=C(C=C2)N=CC3=CC=CC=C3O)O</t>
+          <t>C1=CC(=CC=C1O)O</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="C17" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="D17" t="n">
-        <v>0.0009</v>
+        <v>0.01</v>
       </c>
       <c r="E17" t="n">
         <v>0</v>
       </c>
       <c r="F17" t="n">
-        <v>66.5</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>C1=CC=C(C(=C1)C=NC2=CC=C(C=C2)N=CC3=CC=CC=C3O)O</t>
+          <t>C1=CC(=CC=C1O)O</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="C18" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="D18" t="n">
-        <v>0.0013</v>
+        <v>0.1</v>
       </c>
       <c r="E18" t="n">
         <v>0</v>
       </c>
       <c r="F18" t="n">
-        <v>71.75</v>
+        <v>94.3</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>C1=CC=C(C(=C1)C=NC2=CC=C(C=C2)N=CC3=CC=CC=C3O)O</t>
+          <t>C1=CC=C(C(=C1)O)O</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="C19" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="D19" t="n">
-        <v>0.0016</v>
+        <v>0.001</v>
       </c>
       <c r="E19" t="n">
         <v>0</v>
       </c>
       <c r="F19" t="n">
-        <v>76.625</v>
+        <v>51.7</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>C1=CC=C(C(=C1)C=NC2=CC=C(C=C2)N=CC3=CC=CC=C3O)O</t>
+          <t>C1=CC=C(C(=C1)O)O</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="C20" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="D20" t="n">
-        <v>0.0016</v>
+        <v>0.01</v>
       </c>
       <c r="E20" t="n">
         <v>0</v>
       </c>
       <c r="F20" t="n">
-        <v>83</v>
+        <v>63.2</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>C1=CC=C(C(=C1)C=NC2=CC=C(C=C2)N=CC3=CC=CC=C3O)O</t>
+          <t>C1=CC=C(C(=C1)O)O</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="C21" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="D21" t="n">
-        <v>0.0016</v>
+        <v>0.1</v>
       </c>
       <c r="E21" t="n">
         <v>0</v>
       </c>
       <c r="F21" t="n">
-        <v>79</v>
+        <v>96.2</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>C1=CC=C(C(=C1)C=NC2=CC=C(C=C2)N=CC3=CC=CC=C3O)O</t>
+          <t>C=CCN(CC=C)C1=NC(=NC(=N1)S)S[Na]</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C22" t="n">
-        <v>0</v>
+        <v>0.7</v>
       </c>
       <c r="D22" t="n">
-        <v>0.0016</v>
+        <v>0.002</v>
       </c>
       <c r="E22" t="n">
         <v>0</v>
       </c>
       <c r="F22" t="n">
-        <v>69.5</v>
+        <v>52</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>C1=CC=C(C(=C1)C=NC2=CC=C(C=C2)N=CC3=CC=CC=C3O)O</t>
+          <t>C=CCN(CC=C)C1=NC(=NC(=N1)S)S[Na]</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>24</v>
+        <v>2</v>
       </c>
       <c r="C23" t="n">
         <v>0</v>
       </c>
       <c r="D23" t="n">
-        <v>0.0016</v>
+        <v>1e-05</v>
       </c>
       <c r="E23" t="n">
         <v>0</v>
       </c>
       <c r="F23" t="n">
-        <v>19</v>
+        <v>74.565</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>C=CCN(CC=C)C1=NC(=NC(=N1)S)S[Na]</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>2</v>
+      </c>
+      <c r="C24" t="n">
+        <v>0</v>
+      </c>
+      <c r="D24" t="n">
+        <v>3e-05</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0</v>
+      </c>
+      <c r="F24" t="n">
+        <v>91.59999999999999</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>C=CCN(CC=C)C1=NC(=NC(=N1)S)S[Na]</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>2</v>
+      </c>
+      <c r="C25" t="n">
+        <v>0</v>
+      </c>
+      <c r="D25" t="n">
+        <v>5e-05</v>
+      </c>
+      <c r="E25" t="n">
+        <v>0</v>
+      </c>
+      <c r="F25" t="n">
+        <v>91.73</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>C=CCN(CC=C)C1=NC(=NC(=N1)S)S[Na]</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>2</v>
+      </c>
+      <c r="C26" t="n">
+        <v>0</v>
+      </c>
+      <c r="D26" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="E26" t="n">
+        <v>0</v>
+      </c>
+      <c r="F26" t="n">
+        <v>92.86500000000001</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>C=CCN(CC=C)C1=NC(=NC(=N1)S)S[Na]</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>2</v>
+      </c>
+      <c r="C27" t="n">
+        <v>0</v>
+      </c>
+      <c r="D27" t="n">
+        <v>0.0005</v>
+      </c>
+      <c r="E27" t="n">
+        <v>0</v>
+      </c>
+      <c r="F27" t="n">
+        <v>96.56999999999999</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>C=CCN(CC=C)C1=NC(=NC(=N1)S)S[Na]</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>2</v>
+      </c>
+      <c r="C28" t="n">
+        <v>0</v>
+      </c>
+      <c r="D28" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="E28" t="n">
+        <v>0</v>
+      </c>
+      <c r="F28" t="n">
+        <v>98.16499999999999</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>C=CCN(CC=C)C1=NC(=NC(=N1)S)S[Na]</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>5</v>
+      </c>
+      <c r="C29" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="D29" t="n">
+        <v>0.002</v>
+      </c>
+      <c r="E29" t="n">
+        <v>0</v>
+      </c>
+      <c r="F29" t="n">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>C=CCN(CC=C)C1=NC(=NC(=N1)S)S[Na]</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>10</v>
+      </c>
+      <c r="C30" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="D30" t="n">
+        <v>0.002</v>
+      </c>
+      <c r="E30" t="n">
+        <v>0</v>
+      </c>
+      <c r="F30" t="n">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>C=CCN(CC=C)C1=NC(=NC(=N1)S)S[Na]</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>24</v>
+      </c>
+      <c r="C31" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="D31" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="E31" t="n">
+        <v>0</v>
+      </c>
+      <c r="F31" t="n">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>C=CCN(CC=C)C1=NC(=NC(=N1)S)S[Na]</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>24</v>
+      </c>
+      <c r="C32" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="D32" t="n">
+        <v>0.0005</v>
+      </c>
+      <c r="E32" t="n">
+        <v>0</v>
+      </c>
+      <c r="F32" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>C=CCN(CC=C)C1=NC(=NC(=N1)S)S[Na]</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>24</v>
+      </c>
+      <c r="C33" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="D33" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="E33" t="n">
+        <v>0</v>
+      </c>
+      <c r="F33" t="n">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>C=CCN(CC=C)C1=NC(=NC(=N1)S)S[Na]</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>24</v>
+      </c>
+      <c r="C34" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="D34" t="n">
+        <v>0.0015</v>
+      </c>
+      <c r="E34" t="n">
+        <v>0</v>
+      </c>
+      <c r="F34" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>C=CCN(CC=C)C1=NC(=NC(=N1)S)S[Na]</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>24</v>
+      </c>
+      <c r="C35" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="D35" t="n">
+        <v>0.002</v>
+      </c>
+      <c r="E35" t="n">
+        <v>0</v>
+      </c>
+      <c r="F35" t="n">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>C=CCN(CC=C)C1=NC(=NC(=N1)S)S[Na]</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>24</v>
+      </c>
+      <c r="C36" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="D36" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="E36" t="n">
+        <v>0</v>
+      </c>
+      <c r="F36" t="n">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>C=CCN(CC=C)C1=NC(=NC(=N1)S)S[Na]</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>24</v>
+      </c>
+      <c r="C37" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="D37" t="n">
+        <v>0.0005</v>
+      </c>
+      <c r="E37" t="n">
+        <v>0</v>
+      </c>
+      <c r="F37" t="n">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>C=CCN(CC=C)C1=NC(=NC(=N1)S)S[Na]</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>24</v>
+      </c>
+      <c r="C38" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="D38" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="E38" t="n">
+        <v>0</v>
+      </c>
+      <c r="F38" t="n">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>C=CCN(CC=C)C1=NC(=NC(=N1)S)S[Na]</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>24</v>
+      </c>
+      <c r="C39" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="D39" t="n">
+        <v>0.0015</v>
+      </c>
+      <c r="E39" t="n">
+        <v>0</v>
+      </c>
+      <c r="F39" t="n">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>C=CCN(CC=C)C1=NC(=NC(=N1)S)S[Na]</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>24</v>
+      </c>
+      <c r="C40" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="D40" t="n">
+        <v>0.002</v>
+      </c>
+      <c r="E40" t="n">
+        <v>0</v>
+      </c>
+      <c r="F40" t="n">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>C=CCN(CC=C)C1=NC(=NC(=N1)S)S[Na]</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>24</v>
+      </c>
+      <c r="C41" t="n">
+        <v>7</v>
+      </c>
+      <c r="D41" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="E41" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F41" t="n">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>C=CCN(CC=C)C1=NC(=NC(=N1)S)S[Na]</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>24</v>
+      </c>
+      <c r="C42" t="n">
+        <v>7</v>
+      </c>
+      <c r="D42" t="n">
+        <v>0.0005</v>
+      </c>
+      <c r="E42" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F42" t="n">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>C=CCN(CC=C)C1=NC(=NC(=N1)S)S[Na]</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>24</v>
+      </c>
+      <c r="C43" t="n">
+        <v>7</v>
+      </c>
+      <c r="D43" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="E43" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F43" t="n">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>C=CCN(CC=C)C1=NC(=NC(=N1)S)S[Na]</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
+        <v>24</v>
+      </c>
+      <c r="C44" t="n">
+        <v>7</v>
+      </c>
+      <c r="D44" t="n">
+        <v>0.0015</v>
+      </c>
+      <c r="E44" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F44" t="n">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>C=CCN(CC=C)C1=NC(=NC(=N1)S)S[Na]</t>
+        </is>
+      </c>
+      <c r="B45" t="n">
+        <v>24</v>
+      </c>
+      <c r="C45" t="n">
+        <v>7</v>
+      </c>
+      <c r="D45" t="n">
+        <v>0.002</v>
+      </c>
+      <c r="E45" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F45" t="n">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>C=CCN(CC=C)C1=NC(=NC(=N1)S)S[Na]</t>
+        </is>
+      </c>
+      <c r="B46" t="n">
+        <v>48</v>
+      </c>
+      <c r="C46" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="D46" t="n">
+        <v>0.002</v>
+      </c>
+      <c r="E46" t="n">
+        <v>0</v>
+      </c>
+      <c r="F46" t="n">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>CC1=C(SC=[N+]1CC2=CN=C(N=C2N)C)CCO</t>
+        </is>
+      </c>
+      <c r="B47" t="n">
+        <v>0.67</v>
+      </c>
+      <c r="C47" t="n">
+        <v>0</v>
+      </c>
+      <c r="D47" t="n">
+        <v>0.0008</v>
+      </c>
+      <c r="E47" t="n">
+        <v>0</v>
+      </c>
+      <c r="F47" t="n">
+        <v>85.56999999999999</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>CC1=C(SC=[N+]1CC2=CN=C(N=C2N)C)CCO</t>
+        </is>
+      </c>
+      <c r="B48" t="n">
+        <v>0.67</v>
+      </c>
+      <c r="C48" t="n">
+        <v>0</v>
+      </c>
+      <c r="D48" t="n">
+        <v>0.004</v>
+      </c>
+      <c r="E48" t="n">
+        <v>0</v>
+      </c>
+      <c r="F48" t="n">
+        <v>88.625</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>CC1=C(SC=[N+]1CC2=CN=C(N=C2N)C)CCO</t>
+        </is>
+      </c>
+      <c r="B49" t="n">
+        <v>0.67</v>
+      </c>
+      <c r="C49" t="n">
+        <v>0</v>
+      </c>
+      <c r="D49" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="E49" t="n">
+        <v>0</v>
+      </c>
+      <c r="F49" t="n">
+        <v>89.94</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>CC1=C(SC=[N+]1CC2=CN=C(N=C2N)C)CCO</t>
+        </is>
+      </c>
+      <c r="B50" t="n">
+        <v>0.67</v>
+      </c>
+      <c r="C50" t="n">
+        <v>0</v>
+      </c>
+      <c r="D50" t="n">
+        <v>0.025</v>
+      </c>
+      <c r="E50" t="n">
+        <v>0</v>
+      </c>
+      <c r="F50" t="n">
+        <v>92.1875</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>CC1=C(SC=[N+]1CC2=CN=C(N=C2N)C)CCO</t>
+        </is>
+      </c>
+      <c r="B51" t="n">
+        <v>24</v>
+      </c>
+      <c r="C51" t="n">
+        <v>0</v>
+      </c>
+      <c r="D51" t="n">
+        <v>0.0008</v>
+      </c>
+      <c r="E51" t="n">
+        <v>0</v>
+      </c>
+      <c r="F51" t="n">
+        <v>58.5</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>CC1=C(SC=[N+]1CC2=CN=C(N=C2N)C)CCO</t>
+        </is>
+      </c>
+      <c r="B52" t="n">
+        <v>24</v>
+      </c>
+      <c r="C52" t="n">
+        <v>0</v>
+      </c>
+      <c r="D52" t="n">
+        <v>0.004</v>
+      </c>
+      <c r="E52" t="n">
+        <v>0</v>
+      </c>
+      <c r="F52" t="n">
+        <v>73.75</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>CC1=C(SC=[N+]1CC2=CN=C(N=C2N)C)CCO</t>
+        </is>
+      </c>
+      <c r="B53" t="n">
+        <v>24</v>
+      </c>
+      <c r="C53" t="n">
+        <v>0</v>
+      </c>
+      <c r="D53" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="E53" t="n">
+        <v>0</v>
+      </c>
+      <c r="F53" t="n">
+        <v>79.75</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>CC1=C(SC=[N+]1CC2=CN=C(N=C2N)C)CCO</t>
+        </is>
+      </c>
+      <c r="B54" t="n">
+        <v>24</v>
+      </c>
+      <c r="C54" t="n">
+        <v>0</v>
+      </c>
+      <c r="D54" t="n">
+        <v>0.025</v>
+      </c>
+      <c r="E54" t="n">
+        <v>0</v>
+      </c>
+      <c r="F54" t="n">
+        <v>82.125</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>CCCCN(CCCC)C1=NC(=NC(=N1)S)S[Na]</t>
+        </is>
+      </c>
+      <c r="B55" t="n">
+        <v>2</v>
+      </c>
+      <c r="C55" t="n">
+        <v>0</v>
+      </c>
+      <c r="D55" t="n">
+        <v>1e-05</v>
+      </c>
+      <c r="E55" t="n">
+        <v>0</v>
+      </c>
+      <c r="F55" t="n">
+        <v>50.89</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>CCCCN(CCCC)C1=NC(=NC(=N1)S)S[Na]</t>
+        </is>
+      </c>
+      <c r="B56" t="n">
+        <v>2</v>
+      </c>
+      <c r="C56" t="n">
+        <v>0</v>
+      </c>
+      <c r="D56" t="n">
+        <v>3e-05</v>
+      </c>
+      <c r="E56" t="n">
+        <v>0</v>
+      </c>
+      <c r="F56" t="n">
+        <v>84.25</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>CCCCN(CCCC)C1=NC(=NC(=N1)S)S[Na]</t>
+        </is>
+      </c>
+      <c r="B57" t="n">
+        <v>2</v>
+      </c>
+      <c r="C57" t="n">
+        <v>0</v>
+      </c>
+      <c r="D57" t="n">
+        <v>5e-05</v>
+      </c>
+      <c r="E57" t="n">
+        <v>0</v>
+      </c>
+      <c r="F57" t="n">
+        <v>89.72</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>CCCCN(CCCC)C1=NC(=NC(=N1)S)S[Na]</t>
+        </is>
+      </c>
+      <c r="B58" t="n">
+        <v>2</v>
+      </c>
+      <c r="C58" t="n">
+        <v>0</v>
+      </c>
+      <c r="D58" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="E58" t="n">
+        <v>0</v>
+      </c>
+      <c r="F58" t="n">
+        <v>96.685</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>CCCCN(CCCC)C1=NC(=NC(=N1)S)S[Na]</t>
+        </is>
+      </c>
+      <c r="B59" t="n">
+        <v>2</v>
+      </c>
+      <c r="C59" t="n">
+        <v>0</v>
+      </c>
+      <c r="D59" t="n">
+        <v>0.0005</v>
+      </c>
+      <c r="E59" t="n">
+        <v>0</v>
+      </c>
+      <c r="F59" t="n">
+        <v>98.405</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>CCCCN(CCCC)C1=NC(=NC(=N1)S)S[Na]</t>
+        </is>
+      </c>
+      <c r="B60" t="n">
+        <v>2</v>
+      </c>
+      <c r="C60" t="n">
+        <v>0</v>
+      </c>
+      <c r="D60" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="E60" t="n">
+        <v>0</v>
+      </c>
+      <c r="F60" t="n">
+        <v>99.02</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>COC1=C(C=CC(=C1)C2=CC(=C(C=C2)N=NC3=C(C4=C(C=C(C=C4C=C3S(=O)(=O)[O-])S(=O)(=O)[O-])N)O)OC)N=NC5=C(C6=C(C=C(C=C6C=C5S(=O)(=O)[O-])S(=O)(=O)[O-])N)O.[Na+].[Na+].[Na+].[Na+]</t>
+        </is>
+      </c>
+      <c r="B61" t="n">
+        <v>10</v>
+      </c>
+      <c r="C61" t="n">
+        <v>7</v>
+      </c>
+      <c r="D61" t="n">
+        <v>5e-05</v>
+      </c>
+      <c r="E61" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F61" t="n">
+        <v>66.66499999999999</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>COC1=C(C=CC(=C1)C2=CC(=C(C=C2)N=NC3=C(C4=C(C=C(C=C4C=C3S(=O)(=O)[O-])S(=O)(=O)[O-])N)O)OC)N=NC5=C(C6=C(C=C(C=C6C=C5S(=O)(=O)[O-])S(=O)(=O)[O-])N)O.[Na+].[Na+].[Na+].[Na+]</t>
+        </is>
+      </c>
+      <c r="B62" t="n">
+        <v>10</v>
+      </c>
+      <c r="C62" t="n">
+        <v>7</v>
+      </c>
+      <c r="D62" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="E62" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F62" t="n">
+        <v>74.53</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>COC1=C(C=CC(=C1)C2=CC(=C(C=C2)N=NC3=C(C4=C(C=C(C=C4C=C3S(=O)(=O)[O-])S(=O)(=O)[O-])N)O)OC)N=NC5=C(C6=C(C=C(C=C6C=C5S(=O)(=O)[O-])S(=O)(=O)[O-])N)O.[Na+].[Na+].[Na+].[Na+]</t>
+        </is>
+      </c>
+      <c r="B63" t="n">
+        <v>10</v>
+      </c>
+      <c r="C63" t="n">
+        <v>7</v>
+      </c>
+      <c r="D63" t="n">
+        <v>0.00015</v>
+      </c>
+      <c r="E63" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F63" t="n">
+        <v>85.64</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>COC1=C(C=CC(=C1)C2=CC(=C(C=C2)N=NC3=C(C4=C(C=C(C=C4C=C3S(=O)(=O)[O-])S(=O)(=O)[O-])N)O)OC)N=NC5=C(C6=C(C=C(C=C6C=C5S(=O)(=O)[O-])S(=O)(=O)[O-])N)O.[Na+].[Na+].[Na+].[Na+]</t>
+        </is>
+      </c>
+      <c r="B64" t="n">
+        <v>10</v>
+      </c>
+      <c r="C64" t="n">
+        <v>7</v>
+      </c>
+      <c r="D64" t="n">
+        <v>0.0002</v>
+      </c>
+      <c r="E64" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F64" t="n">
+        <v>90.67</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>NC(CO)C(=O)O</t>
+        </is>
+      </c>
+      <c r="B65" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="C65" t="n">
+        <v>11</v>
+      </c>
+      <c r="D65" t="n">
+        <v>0.0045</v>
+      </c>
+      <c r="E65" t="n">
+        <v>0</v>
+      </c>
+      <c r="F65" t="n">
+        <v>50.4</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>NC(CO)C(=O)O</t>
+        </is>
+      </c>
+      <c r="B66" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="C66" t="n">
+        <v>11</v>
+      </c>
+      <c r="D66" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="E66" t="n">
+        <v>0</v>
+      </c>
+      <c r="F66" t="n">
+        <v>63.25</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>NC(CO)C(=O)O</t>
+        </is>
+      </c>
+      <c r="B67" t="n">
+        <v>0.58</v>
+      </c>
+      <c r="C67" t="n">
+        <v>11</v>
+      </c>
+      <c r="D67" t="n">
+        <v>0.0045</v>
+      </c>
+      <c r="E67" t="n">
+        <v>0</v>
+      </c>
+      <c r="F67" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>NC(CO)C(=O)O</t>
+        </is>
+      </c>
+      <c r="B68" t="n">
+        <v>1.67</v>
+      </c>
+      <c r="C68" t="n">
+        <v>11</v>
+      </c>
+      <c r="D68" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="E68" t="n">
+        <v>0</v>
+      </c>
+      <c r="F68" t="n">
+        <v>61.3</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>O=C(O)/C=C\C(=O)O</t>
+        </is>
+      </c>
+      <c r="B69" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="C69" t="n">
+        <v>11</v>
+      </c>
+      <c r="D69" t="n">
+        <v>0.0045</v>
+      </c>
+      <c r="E69" t="n">
+        <v>0</v>
+      </c>
+      <c r="F69" t="n">
+        <v>64.3</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>O=C(O)/C=C\C(=O)O</t>
+        </is>
+      </c>
+      <c r="B70" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="C70" t="n">
+        <v>11</v>
+      </c>
+      <c r="D70" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="E70" t="n">
+        <v>0</v>
+      </c>
+      <c r="F70" t="n">
+        <v>99.05</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>O=C(O)/C=C\C(=O)O</t>
+        </is>
+      </c>
+      <c r="B71" t="n">
+        <v>0.58</v>
+      </c>
+      <c r="C71" t="n">
+        <v>11</v>
+      </c>
+      <c r="D71" t="n">
+        <v>0.0045</v>
+      </c>
+      <c r="E71" t="n">
+        <v>0</v>
+      </c>
+      <c r="F71" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>O=C(O)/C=C\C(=O)O</t>
+        </is>
+      </c>
+      <c r="B72" t="n">
+        <v>1.67</v>
+      </c>
+      <c r="C72" t="n">
+        <v>11</v>
+      </c>
+      <c r="D72" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="E72" t="n">
+        <v>0</v>
+      </c>
+      <c r="F72" t="n">
+        <v>99.7</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>O=C(O)C(O)C(O)C(=O)O</t>
+        </is>
+      </c>
+      <c r="B73" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="C73" t="n">
+        <v>11</v>
+      </c>
+      <c r="D73" t="n">
+        <v>0.0045</v>
+      </c>
+      <c r="E73" t="n">
+        <v>0</v>
+      </c>
+      <c r="F73" t="n">
+        <v>71.59999999999999</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>O=C(O)C(O)C(O)C(=O)O</t>
+        </is>
+      </c>
+      <c r="B74" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="C74" t="n">
+        <v>11</v>
+      </c>
+      <c r="D74" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="E74" t="n">
+        <v>0</v>
+      </c>
+      <c r="F74" t="n">
+        <v>98.45</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>O=C(O)C(O)C(O)C(=O)O</t>
+        </is>
+      </c>
+      <c r="B75" t="n">
+        <v>0.58</v>
+      </c>
+      <c r="C75" t="n">
+        <v>11</v>
+      </c>
+      <c r="D75" t="n">
+        <v>0.0045</v>
+      </c>
+      <c r="E75" t="n">
+        <v>0</v>
+      </c>
+      <c r="F75" t="n">
+        <v>45.5</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>O=C(O)C(O)C(O)C(=O)O</t>
+        </is>
+      </c>
+      <c r="B76" t="n">
+        <v>1.67</v>
+      </c>
+      <c r="C76" t="n">
+        <v>11</v>
+      </c>
+      <c r="D76" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="E76" t="n">
+        <v>0</v>
+      </c>
+      <c r="F76" t="n">
+        <v>99.40000000000001</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>O=C(O)CC(CC(=O)O)C(=O)O</t>
+        </is>
+      </c>
+      <c r="B77" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="C77" t="n">
+        <v>11</v>
+      </c>
+      <c r="D77" t="n">
+        <v>0.0045</v>
+      </c>
+      <c r="E77" t="n">
+        <v>0</v>
+      </c>
+      <c r="F77" t="n">
+        <v>81.55</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>O=C(O)CC(CC(=O)O)C(=O)O</t>
+        </is>
+      </c>
+      <c r="B78" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="C78" t="n">
+        <v>11</v>
+      </c>
+      <c r="D78" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="E78" t="n">
+        <v>0</v>
+      </c>
+      <c r="F78" t="n">
+        <v>99.7</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>O=C(O)CC(CC(=O)O)C(=O)O</t>
+        </is>
+      </c>
+      <c r="B79" t="n">
+        <v>0.58</v>
+      </c>
+      <c r="C79" t="n">
+        <v>11</v>
+      </c>
+      <c r="D79" t="n">
+        <v>0.0045</v>
+      </c>
+      <c r="E79" t="n">
+        <v>0</v>
+      </c>
+      <c r="F79" t="n">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>O=C(O)CC(CC(=O)O)C(=O)O</t>
+        </is>
+      </c>
+      <c r="B80" t="n">
+        <v>1.67</v>
+      </c>
+      <c r="C80" t="n">
+        <v>11</v>
+      </c>
+      <c r="D80" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="E80" t="n">
+        <v>0</v>
+      </c>
+      <c r="F80" t="n">
+        <v>99.7</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>O=C(O)CC(O)C(=O)O</t>
+        </is>
+      </c>
+      <c r="B81" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="C81" t="n">
+        <v>11</v>
+      </c>
+      <c r="D81" t="n">
+        <v>0.0045</v>
+      </c>
+      <c r="E81" t="n">
+        <v>0</v>
+      </c>
+      <c r="F81" t="n">
+        <v>60.75</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>O=C(O)CC(O)C(=O)O</t>
+        </is>
+      </c>
+      <c r="B82" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="C82" t="n">
+        <v>11</v>
+      </c>
+      <c r="D82" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="E82" t="n">
+        <v>0</v>
+      </c>
+      <c r="F82" t="n">
+        <v>97.90000000000001</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>O=C(O)CC(O)C(=O)O</t>
+        </is>
+      </c>
+      <c r="B83" t="n">
+        <v>0.58</v>
+      </c>
+      <c r="C83" t="n">
+        <v>11</v>
+      </c>
+      <c r="D83" t="n">
+        <v>0.0045</v>
+      </c>
+      <c r="E83" t="n">
+        <v>0</v>
+      </c>
+      <c r="F83" t="n">
+        <v>33.3</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>O=C(O)CC(O)C(=O)O</t>
+        </is>
+      </c>
+      <c r="B84" t="n">
+        <v>1.67</v>
+      </c>
+      <c r="C84" t="n">
+        <v>11</v>
+      </c>
+      <c r="D84" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="E84" t="n">
+        <v>0</v>
+      </c>
+      <c r="F84" t="n">
+        <v>99.2</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>O=C(O)CCC(=O)O</t>
+        </is>
+      </c>
+      <c r="B85" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="C85" t="n">
+        <v>11</v>
+      </c>
+      <c r="D85" t="n">
+        <v>0.0045</v>
+      </c>
+      <c r="E85" t="n">
+        <v>0</v>
+      </c>
+      <c r="F85" t="n">
+        <v>62.75</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>O=C(O)CCC(=O)O</t>
+        </is>
+      </c>
+      <c r="B86" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="C86" t="n">
+        <v>11</v>
+      </c>
+      <c r="D86" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="E86" t="n">
+        <v>0</v>
+      </c>
+      <c r="F86" t="n">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>O=C(O)CCC(=O)O</t>
+        </is>
+      </c>
+      <c r="B87" t="n">
+        <v>0.58</v>
+      </c>
+      <c r="C87" t="n">
+        <v>11</v>
+      </c>
+      <c r="D87" t="n">
+        <v>0.0045</v>
+      </c>
+      <c r="E87" t="n">
+        <v>0</v>
+      </c>
+      <c r="F87" t="n">
+        <v>47.8</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>O=C(O)CCC(=O)O</t>
+        </is>
+      </c>
+      <c r="B88" t="n">
+        <v>1.67</v>
+      </c>
+      <c r="C88" t="n">
+        <v>11</v>
+      </c>
+      <c r="D88" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="E88" t="n">
+        <v>0</v>
+      </c>
+      <c r="F88" t="n">
+        <v>99.8</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>OC(=O)C(CC(=O)O)(CC(=O)O)O</t>
+        </is>
+      </c>
+      <c r="B89" t="n">
+        <v>1.67</v>
+      </c>
+      <c r="C89" t="n">
+        <v>11</v>
+      </c>
+      <c r="D89" t="n">
+        <v>0.002</v>
+      </c>
+      <c r="E89" t="n">
+        <v>0</v>
+      </c>
+      <c r="F89" t="n">
+        <v>83.91666666666667</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>Oc1cccc2c1nccc2</t>
+        </is>
+      </c>
+      <c r="B90" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C90" t="n">
+        <v>13.7</v>
+      </c>
+      <c r="D90" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="E90" t="n">
+        <v>0</v>
+      </c>
+      <c r="F90" t="n">
+        <v>10.025</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>Oc1cccc2c1nccc2</t>
+        </is>
+      </c>
+      <c r="B91" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C91" t="n">
+        <v>14.30102999566398</v>
+      </c>
+      <c r="D91" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="E91" t="n">
+        <v>0</v>
+      </c>
+      <c r="F91" t="n">
+        <v>11.55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>